<commit_message>
config changed, factor adjustment per meal type
</commit_message>
<xml_diff>
--- a/resources/config/binge_config.xlsx
+++ b/resources/config/binge_config.xlsx
@@ -1,30 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\nlp-datau\resources\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanderputs/Documents/git/psych-datau/resources/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{275FC518-C1F2-7340-8EA5-8A4FC64DC2FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
   <si>
     <t>#</t>
   </si>
@@ -153,13 +162,37 @@
   </si>
   <si>
     <t>other_int</t>
+  </si>
+  <si>
+    <t>N.B. It depends if you go for volle, halfvolle, magere yoghurt… I chose halfvolle but it is very random</t>
+  </si>
+  <si>
+    <t>again: volkoren, witte brood, zoutarm…</t>
+  </si>
+  <si>
+    <t>erg moeilijk want er is maaltijdsalade vs. sla so what to choose?</t>
+  </si>
+  <si>
+    <t>calories</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>other_factor</t>
+  </si>
+  <si>
+    <t>meals_factor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,6 +230,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -206,7 +245,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -266,11 +305,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -305,6 +353,16 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,16 +642,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="8" max="8" width="15.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="1" spans="1:11" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -615,8 +677,20 @@
       <c r="G1" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="32.75" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="H1" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -638,8 +712,19 @@
       <c r="G2" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="64.75" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="H2" s="15">
+        <f>1/(SUM(F2,1))</f>
+        <v>0.2</v>
+      </c>
+      <c r="I2" s="15">
+        <f>1/(SUM(G2,1))</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J2" s="13">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="69" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>2</v>
       </c>
@@ -661,8 +746,19 @@
       <c r="G3" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="64.75" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="H3" s="15">
+        <f t="shared" ref="H3:H25" si="0">1/(SUM(F3,1))</f>
+        <v>0.5</v>
+      </c>
+      <c r="I3" s="15">
+        <f t="shared" ref="I3:I25" si="1">1/(SUM(G3,1))</f>
+        <v>0.5</v>
+      </c>
+      <c r="J3" s="13">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="69" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>3</v>
       </c>
@@ -684,8 +780,22 @@
       <c r="G4" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="16.75" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="H4" s="15">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="I4" s="15">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="J4" s="13">
+        <v>75</v>
+      </c>
+      <c r="K4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>4</v>
       </c>
@@ -707,8 +817,19 @@
       <c r="G5" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="H5" s="15">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I5" s="15">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J5" s="13">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>5</v>
       </c>
@@ -730,8 +851,19 @@
       <c r="G6" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="64.75" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="H6" s="15">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I6" s="15">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="J6" s="13">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>6</v>
       </c>
@@ -753,8 +885,22 @@
       <c r="G7" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="64.75" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="H7" s="15">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I7" s="15">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="J7" s="13">
+        <v>85</v>
+      </c>
+      <c r="K7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="69" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>7</v>
       </c>
@@ -776,8 +922,19 @@
       <c r="G8" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="16.75" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="H8" s="15">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I8" s="15">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="J8" s="13">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>8</v>
       </c>
@@ -799,8 +956,22 @@
       <c r="G9" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="112.75" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="H9" s="15">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I9" s="15">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="J9" s="13">
+        <v>175</v>
+      </c>
+      <c r="K9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="120" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -822,8 +993,19 @@
       <c r="G10" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="32.75" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="H10" s="15">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="I10" s="15">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J10" s="13">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -845,8 +1027,19 @@
       <c r="G11" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="32.75" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="H11" s="15">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I11" s="15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J11" s="13">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -868,8 +1061,19 @@
       <c r="G12" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="16.75" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="H12" s="15">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I12" s="15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J12" s="13">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -891,8 +1095,19 @@
       <c r="G13" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="16.75" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="H13" s="15">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I13" s="15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J13" s="13">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>13</v>
       </c>
@@ -914,8 +1129,19 @@
       <c r="G14" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="16.75" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="H14" s="15">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="I14" s="15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J14" s="13">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
         <v>14</v>
       </c>
@@ -937,8 +1163,19 @@
       <c r="G15" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="H15" s="15">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I15" s="15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J15" s="13">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>15</v>
       </c>
@@ -960,8 +1197,19 @@
       <c r="G16" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="112.75" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="H16" s="15">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I16" s="15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J16" s="13">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="120" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>16</v>
       </c>
@@ -983,8 +1231,19 @@
       <c r="G17" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="112.75" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="H17" s="15">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I17" s="15">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J17" s="13">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="120" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>17</v>
       </c>
@@ -1006,8 +1265,19 @@
       <c r="G18" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="112.75" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="H18" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I18" s="15">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J18" s="13">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="120" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
         <v>18</v>
       </c>
@@ -1029,8 +1299,19 @@
       <c r="G19" s="9">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="32.75" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="H19" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I19" s="15">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J19" s="13">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>19</v>
       </c>
@@ -1052,8 +1333,19 @@
       <c r="G20" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="112.75" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="H20" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I20" s="15">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="J20" s="13">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="120" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <v>20</v>
       </c>
@@ -1075,8 +1367,19 @@
       <c r="G21" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="16.75" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="H21" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I21" s="15">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J21" s="13">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
         <v>21</v>
       </c>
@@ -1098,8 +1401,19 @@
       <c r="G22" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="H22" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I22" s="15">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="J22" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
         <v>22</v>
       </c>
@@ -1121,8 +1435,19 @@
       <c r="G23" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="112.75" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="H23" s="15">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="I23" s="15">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="J23" s="13">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="120" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>23</v>
       </c>
@@ -1144,8 +1469,19 @@
       <c r="G24" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="112.75" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="H24" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I24" s="15">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J24" s="13">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="120" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>24</v>
       </c>
@@ -1167,11 +1503,23 @@
       <c r="G25" s="8">
         <v>2</v>
       </c>
+      <c r="H25" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I25" s="15">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J25" s="13">
+        <v>161</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="A2:G25">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G25">
     <sortCondition ref="A1"/>
   </sortState>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
config added removed +1 for threshold in config
</commit_message>
<xml_diff>
--- a/resources/config/binge_config.xlsx
+++ b/resources/config/binge_config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanderputs/Documents/git/psych-datau/resources/config/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/verenajirgal/git/psych-datau/resources/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{275FC518-C1F2-7340-8EA5-8A4FC64DC2FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79AB7EDF-52A2-D148-AC93-E40AB7C0BE24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -646,7 +646,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -713,12 +713,12 @@
         <v>2</v>
       </c>
       <c r="H2" s="15">
-        <f>1/(SUM(F2,1))</f>
-        <v>0.2</v>
+        <f>IFERROR(1/F2,0)</f>
+        <v>0.25</v>
       </c>
       <c r="I2" s="15">
-        <f>1/(SUM(G2,1))</f>
-        <v>0.33333333333333331</v>
+        <f>IFERROR(1/G2,0)</f>
+        <v>0.5</v>
       </c>
       <c r="J2" s="13">
         <v>38</v>
@@ -747,12 +747,12 @@
         <v>1</v>
       </c>
       <c r="H3" s="15">
-        <f t="shared" ref="H3:H25" si="0">1/(SUM(F3,1))</f>
-        <v>0.5</v>
+        <f t="shared" ref="H3:H25" si="0">IFERROR(1/F3,0)</f>
+        <v>1</v>
       </c>
       <c r="I3" s="15">
-        <f t="shared" ref="I3:I25" si="1">1/(SUM(G3,1))</f>
-        <v>0.5</v>
+        <f t="shared" ref="I3:I25" si="1">IFERROR(1/G3,0)</f>
+        <v>1</v>
       </c>
       <c r="J3" s="13">
         <v>158</v>
@@ -782,11 +782,11 @@
       </c>
       <c r="H4" s="15">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="I4" s="15">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J4" s="13">
         <v>75</v>
@@ -819,11 +819,11 @@
       </c>
       <c r="H5" s="15">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="I5" s="15">
         <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="J5" s="13">
         <v>55</v>
@@ -853,11 +853,11 @@
       </c>
       <c r="H6" s="15">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="I6" s="15">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J6" s="13">
         <v>90</v>
@@ -887,11 +887,11 @@
       </c>
       <c r="H7" s="15">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="I7" s="15">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J7" s="13">
         <v>85</v>
@@ -924,11 +924,11 @@
       </c>
       <c r="H8" s="15">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="I8" s="15">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J8" s="13">
         <v>78</v>
@@ -958,11 +958,11 @@
       </c>
       <c r="H9" s="15">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="I9" s="15">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J9" s="13">
         <v>175</v>
@@ -995,11 +995,11 @@
       </c>
       <c r="H10" s="15">
         <f t="shared" si="0"/>
-        <v>0.25</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="I10" s="15">
         <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="J10" s="13">
         <v>14</v>
@@ -1029,11 +1029,11 @@
       </c>
       <c r="H11" s="15">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="I11" s="15">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11" s="13">
         <v>468</v>
@@ -1063,11 +1063,11 @@
       </c>
       <c r="H12" s="15">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="I12" s="15">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" s="13">
         <v>500</v>
@@ -1097,11 +1097,11 @@
       </c>
       <c r="H13" s="15">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="I13" s="15">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" s="13">
         <v>639</v>
@@ -1131,11 +1131,11 @@
       </c>
       <c r="H14" s="15">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="I14" s="15">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" s="13">
         <v>812</v>
@@ -1165,11 +1165,11 @@
       </c>
       <c r="H15" s="15">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="I15" s="15">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15" s="13">
         <v>227</v>
@@ -1199,11 +1199,11 @@
       </c>
       <c r="H16" s="15">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="I16" s="15">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" s="13">
         <v>393</v>
@@ -1233,11 +1233,11 @@
       </c>
       <c r="H17" s="15">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="I17" s="15">
         <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="J17" s="13">
         <v>102</v>
@@ -1267,11 +1267,11 @@
       </c>
       <c r="H18" s="15">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I18" s="15">
         <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="J18" s="13">
         <v>87</v>
@@ -1301,11 +1301,11 @@
       </c>
       <c r="H19" s="15">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I19" s="15">
         <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="J19" s="13">
         <v>214</v>
@@ -1335,11 +1335,11 @@
       </c>
       <c r="H20" s="15">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20" s="15">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J20" s="13">
         <v>219</v>
@@ -1369,11 +1369,11 @@
       </c>
       <c r="H21" s="15">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I21" s="15">
         <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="J21" s="13">
         <v>50</v>
@@ -1403,11 +1403,11 @@
       </c>
       <c r="H22" s="15">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I22" s="15">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J22" s="13">
         <v>200</v>
@@ -1437,11 +1437,11 @@
       </c>
       <c r="H23" s="15">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="I23" s="15">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J23" s="13">
         <v>106</v>
@@ -1471,11 +1471,11 @@
       </c>
       <c r="H24" s="15">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I24" s="15">
         <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="J24" s="13">
         <v>215</v>
@@ -1505,11 +1505,11 @@
       </c>
       <c r="H25" s="15">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I25" s="15">
         <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="J25" s="13">
         <v>161</v>

</xml_diff>

<commit_message>
again change if div 0 its binge in config
</commit_message>
<xml_diff>
--- a/resources/config/binge_config.xlsx
+++ b/resources/config/binge_config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/verenajirgal/git/psych-datau/resources/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79AB7EDF-52A2-D148-AC93-E40AB7C0BE24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDFD6AAD-2A64-7444-8326-0021FBBB8304}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -645,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -713,11 +713,11 @@
         <v>2</v>
       </c>
       <c r="H2" s="15">
-        <f>IFERROR(1/F2,0)</f>
+        <f>IFERROR(1/F2,2)</f>
         <v>0.25</v>
       </c>
       <c r="I2" s="15">
-        <f>IFERROR(1/G2,0)</f>
+        <f>IFERROR(1/G2,2)</f>
         <v>0.5</v>
       </c>
       <c r="J2" s="13">
@@ -747,11 +747,11 @@
         <v>1</v>
       </c>
       <c r="H3" s="15">
-        <f t="shared" ref="H3:H25" si="0">IFERROR(1/F3,0)</f>
+        <f t="shared" ref="H3:H25" si="0">IFERROR(1/F3,2)</f>
         <v>1</v>
       </c>
       <c r="I3" s="15">
-        <f t="shared" ref="I3:I25" si="1">IFERROR(1/G3,0)</f>
+        <f t="shared" ref="I3:I25" si="1">IFERROR(1/G3,2)</f>
         <v>1</v>
       </c>
       <c r="J3" s="13">
@@ -1033,7 +1033,7 @@
       </c>
       <c r="I11" s="15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J11" s="13">
         <v>468</v>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="I12" s="15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J12" s="13">
         <v>500</v>
@@ -1101,7 +1101,7 @@
       </c>
       <c r="I13" s="15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J13" s="13">
         <v>639</v>
@@ -1135,7 +1135,7 @@
       </c>
       <c r="I14" s="15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J14" s="13">
         <v>812</v>
@@ -1169,7 +1169,7 @@
       </c>
       <c r="I15" s="15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J15" s="13">
         <v>227</v>
@@ -1203,7 +1203,7 @@
       </c>
       <c r="I16" s="15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J16" s="13">
         <v>393</v>
@@ -1267,7 +1267,7 @@
       </c>
       <c r="H18" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I18" s="15">
         <f t="shared" si="1"/>
@@ -1301,7 +1301,7 @@
       </c>
       <c r="H19" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I19" s="15">
         <f t="shared" si="1"/>
@@ -1335,7 +1335,7 @@
       </c>
       <c r="H20" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I20" s="15">
         <f t="shared" si="1"/>
@@ -1369,7 +1369,7 @@
       </c>
       <c r="H21" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I21" s="15">
         <f t="shared" si="1"/>
@@ -1403,7 +1403,7 @@
       </c>
       <c r="H22" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I22" s="15">
         <f t="shared" si="1"/>
@@ -1471,7 +1471,7 @@
       </c>
       <c r="H24" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I24" s="15">
         <f t="shared" si="1"/>
@@ -1505,7 +1505,7 @@
       </c>
       <c r="H25" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I25" s="15">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
should be ok now
</commit_message>
<xml_diff>
--- a/resources/config/binge_config.xlsx
+++ b/resources/config/binge_config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/verenajirgal/git/psych-datau/resources/config/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanderputs/Documents/git/psych-datau/resources/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE7FC8BB-F0BA-8C4A-8066-72ED356BF95A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281ED24B-513E-4541-9B33-DD3CEAA6A66B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -645,12 +645,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
     <col min="8" max="8" width="15.33203125" customWidth="1"/>
     <col min="9" max="9" width="18.33203125" customWidth="1"/>
   </cols>
@@ -678,10 +679,10 @@
         <v>42</v>
       </c>
       <c r="H1" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" t="s">
         <v>48</v>
-      </c>
-      <c r="I1" t="s">
-        <v>49</v>
       </c>
       <c r="J1" s="12" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
config changed and bug fixed from "objective_binge_single_cat"
</commit_message>
<xml_diff>
--- a/resources/config/binge_config.xlsx
+++ b/resources/config/binge_config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanderputs/Documents/git/psych-datau/resources/config/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/verenajirgal/git/psych-datau/resources/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281ED24B-513E-4541-9B33-DD3CEAA6A66B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94BE0E2F-BB35-5146-B269-A380D1DF0399}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -645,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -819,12 +819,10 @@
         <v>2</v>
       </c>
       <c r="H5" s="15">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="I5" s="15">
-        <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="J5" s="13">
         <v>55</v>
@@ -958,12 +956,10 @@
         <v>1</v>
       </c>
       <c r="H9" s="15">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="I9" s="15">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J9" s="13">
         <v>175</v>
@@ -995,12 +991,10 @@
         <v>2</v>
       </c>
       <c r="H10" s="15">
-        <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.1666</v>
       </c>
       <c r="I10" s="15">
-        <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="J10" s="13">
         <v>14</v>

</xml_diff>